<commit_message>
Adicionado o node local e azure
</commit_message>
<xml_diff>
--- a/Projeto-Documentacao/Planilhas/aula_marise.xlsx
+++ b/Projeto-Documentacao/Planilhas/aula_marise.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\grupo3-sa\Projeto-Documentacao\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Desktop\grupo3-sa\Projeto-Documentacao\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3142617-7CC7-4DF8-82A2-01F931E959DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A6057F-9083-4E80-BA7A-405F43222640}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>MIN</t>
   </si>
@@ -100,9 +99,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,178 +384,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:L26"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="5" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <v>21.5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <v>22.6</v>
-      </c>
-      <c r="G6" s="1">
-        <f>MIN(E5:E24)</f>
-        <v>19</v>
-      </c>
-      <c r="H6" s="1">
-        <f>QUARTILE(E5:E26,1)</f>
-        <v>21.424999999999997</v>
-      </c>
-      <c r="I6" s="1">
-        <f>AVERAGE(E5:E26)</f>
-        <v>22.245454545454542</v>
-      </c>
-      <c r="J6" s="1">
-        <f>MEDIAN(E5:E26)</f>
-        <v>22.5</v>
-      </c>
-      <c r="K6" s="1">
-        <f>QUARTILE(E5:E26,3)</f>
-        <v>23.4</v>
-      </c>
-      <c r="L6" s="1">
-        <f>MAX(E5:E26)</f>
-        <v>24.3</v>
-      </c>
-    </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <v>20.399999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <v>21.4</v>
-      </c>
-    </row>
-    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E9">
-        <v>21.9</v>
-      </c>
-    </row>
-    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E10">
-        <v>23.9</v>
-      </c>
-    </row>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E11">
-        <v>22.4</v>
-      </c>
-    </row>
-    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E12">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <v>21.6</v>
-      </c>
-    </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E15">
-        <v>22.9</v>
-      </c>
-    </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E16">
-        <v>23.6</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17">
-        <v>22.7</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18">
-        <v>24.3</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19">
-        <v>21.4</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20">
-        <v>22.8</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21">
-        <v>23.4</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22">
-        <v>21.4</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23">
-        <v>23.4</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24">
-        <v>23.4</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26">
-        <v>23.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,29 +408,29 @@
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>17.100000000000001</v>
       </c>
-      <c r="C3" s="2">
-        <f>B3-15</f>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C23" si="0">B3-15</f>
         <v>2.1000000000000014</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M3">
@@ -628,37 +459,37 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>18</v>
       </c>
-      <c r="C4" s="2">
-        <f>B4-15</f>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f>MIN(B3:B23)</f>
         <v>17.100000000000001</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f>QUARTILE(B3:B23,1)</f>
         <v>18.5</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <f>AVERAGE(B3:B23)</f>
         <v>19.595238095238095</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f>MEDIAN(B3:B23)</f>
         <v>19.2</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <f>QUARTILE(B3:B23,3)</f>
         <v>21</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <f>MAX(B3:B23)</f>
         <v>22.1</v>
       </c>
@@ -679,7 +510,7 @@
         <f>QUARTILE(M3:M23,)</f>
         <v>44.5</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="1">
         <f>AVERAGE(M3:M23)</f>
         <v>50.25238095238096</v>
       </c>
@@ -697,37 +528,37 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>18.399999999999999</v>
       </c>
-      <c r="C5" s="2">
-        <f>B5-15</f>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
         <v>3.3999999999999986</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <f>MIN(C3:C23)</f>
         <v>2.1000000000000014</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f>QUARTILE(C3:C23,1)</f>
         <v>3.5</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <f>AVERAGE(C3:C23)</f>
         <v>4.5952380952380949</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f>MEDIAN(C3:C23)</f>
         <v>4.1999999999999993</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <f>QUARTILE(C3:C23,)</f>
         <v>2.1000000000000014</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <f>MAX(C3:C23)</f>
         <v>7.1000000000000014</v>
       </c>
@@ -748,7 +579,7 @@
         <f>QUARTILE(N3:N23,1)</f>
         <v>50.5</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="1">
         <f>AVERAGE(N3:N23)</f>
         <v>54.276190476190486</v>
       </c>
@@ -766,14 +597,14 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>18.5</v>
       </c>
-      <c r="C6" s="2">
-        <f>B6-15</f>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="1"/>
       <c r="M6">
         <v>48.8</v>
       </c>
@@ -782,14 +613,14 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>18.600000000000001</v>
       </c>
-      <c r="C7" s="2">
-        <f>B7-15</f>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
         <v>3.6000000000000014</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="1"/>
       <c r="M7">
         <v>49.1</v>
       </c>
@@ -798,14 +629,14 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>19.100000000000001</v>
       </c>
-      <c r="C8" s="2">
-        <f>B8-15</f>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
         <v>4.1000000000000014</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="1"/>
       <c r="M8">
         <v>50.9</v>
       </c>
@@ -814,14 +645,14 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>19.2</v>
       </c>
-      <c r="C9" s="2">
-        <f>B9-15</f>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
         <v>4.1999999999999993</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="1"/>
       <c r="M9">
         <v>49.6</v>
       </c>
@@ -830,15 +661,15 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>19.3</v>
       </c>
-      <c r="C10" s="2">
-        <f>B10-15</f>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
         <v>4.3000000000000007</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="F10" s="1"/>
+      <c r="L10" s="1"/>
       <c r="M10">
         <v>55.5</v>
       </c>
@@ -847,14 +678,14 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>20</v>
       </c>
-      <c r="C11" s="2">
-        <f>B11-15</f>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="1"/>
       <c r="M11">
         <v>53.2</v>
       </c>
@@ -863,14 +694,14 @@
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>21</v>
       </c>
-      <c r="C12" s="2">
-        <f>B12-15</f>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="1"/>
       <c r="M12">
         <v>57.4</v>
       </c>
@@ -879,14 +710,14 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>20.3</v>
       </c>
-      <c r="C13" s="2">
-        <f>B13-15</f>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
         <v>5.3000000000000007</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="1"/>
       <c r="M13">
         <v>55</v>
       </c>
@@ -895,14 +726,14 @@
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>20.399999999999999</v>
       </c>
-      <c r="C14" s="2">
-        <f>B14-15</f>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
         <v>5.3999999999999986</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="1"/>
       <c r="M14">
         <v>60.2</v>
       </c>
@@ -911,14 +742,14 @@
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>22</v>
       </c>
-      <c r="C15" s="2">
-        <f>B15-15</f>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="1"/>
       <c r="M15">
         <v>53.1</v>
       </c>
@@ -927,14 +758,14 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>21</v>
       </c>
-      <c r="C16" s="2">
-        <f>B16-15</f>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="1"/>
       <c r="M16">
         <v>48.7</v>
       </c>
@@ -943,14 +774,14 @@
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>22.1</v>
       </c>
-      <c r="C17" s="2">
-        <f>B17-15</f>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
         <v>7.1000000000000014</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="1"/>
       <c r="M17">
         <v>44.8</v>
       </c>
@@ -959,14 +790,14 @@
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>21.6</v>
       </c>
-      <c r="C18" s="2">
-        <f>B18-15</f>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
         <v>6.6000000000000014</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="1"/>
       <c r="M18">
         <v>46.3</v>
       </c>
@@ -975,14 +806,14 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>21.7</v>
       </c>
-      <c r="C19" s="2">
-        <f>B19-15</f>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
         <v>6.6999999999999993</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="1"/>
       <c r="M19">
         <v>47.7</v>
       </c>
@@ -991,14 +822,14 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>19</v>
       </c>
-      <c r="C20" s="2">
-        <f>B20-15</f>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="1"/>
       <c r="M20">
         <v>46.5</v>
       </c>
@@ -1007,14 +838,14 @@
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
-        <f>B21-15</f>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="1"/>
       <c r="M21">
         <v>50.1</v>
       </c>
@@ -1023,14 +854,14 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>17.5</v>
       </c>
-      <c r="C22" s="2">
-        <f>B22-15</f>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="1"/>
       <c r="M22">
         <v>50.5</v>
       </c>
@@ -1039,14 +870,14 @@
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>18.7</v>
       </c>
-      <c r="C23" s="2">
-        <f>B23-15</f>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
         <v>3.6999999999999993</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="1"/>
       <c r="M23">
         <v>51.9</v>
       </c>

</xml_diff>